<commit_message>
feat: Add synchronized billing audit system to workflow
- Enhanced YAML workflow to run audit system after Excel generation
- Added comprehensive billing audit system with historical data protection
- Implemented smart filtering to only flag unauthorized past-week changes
- Added Sheet Reference column with direct Smartsheet URLs for investigation
- Integrated Delta calculation for financial impact assessment
- Updated workflow name to 'Excel Generation & Billing Audit System'
- Both systems now run synchronously every 2 hours
- Added audit system documentation and setup instructions
- Enhanced logging to show both systems in execution summary

New Features:
 Historical data protection monitoring
 Direct sheet reference links for violations
 Financial impact tracking via Delta column
 Smart filtering ignores current week changes
 Synchronized execution with Excel generation

Ready for production deployment with AUDIT_SHEET_ID secret configuration.
</commit_message>
<xml_diff>
--- a/generated_docs/WR_89699991_WeekEnding_072725.xlsx
+++ b/generated_docs/WR_89699991_WeekEnding_072725.xlsx
@@ -571,7 +571,7 @@
     <row r="5">
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>Report Generated On: 07/30/2025 01:48 PM</t>
+          <t>Report Generated On: 08/16/2025 12:48 AM</t>
         </is>
       </c>
     </row>
@@ -603,7 +603,7 @@
       </c>
       <c r="G8" s="6" t="inlineStr">
         <is>
-          <t>Bryant Murphy</t>
+          <t>JH</t>
         </is>
       </c>
     </row>
@@ -635,7 +635,7 @@
       </c>
       <c r="C10" s="6" t="inlineStr">
         <is>
-          <t>07/27/2025 to 07/27/25</t>
+          <t>07/21/2025 to 07/27/25</t>
         </is>
       </c>
       <c r="F10" s="4" t="inlineStr">
@@ -681,7 +681,7 @@
       </c>
       <c r="G13" s="6" t="inlineStr">
         <is>
-          <t>846-2</t>
+          <t>704-2</t>
         </is>
       </c>
     </row>

</xml_diff>